<commit_message>
Co-authored-by: aFarisk <aFarisk@users.noreply.github.com> Co-authored-by: robby.juliantino@outlook.com <robby.juliantino@outlook.com>
</commit_message>
<xml_diff>
--- a/website/static/VisitorApprovalBT.xlsx
+++ b/website/static/VisitorApprovalBT.xlsx
@@ -966,7 +966,7 @@
       <c r="B6" s="34" t="n"/>
       <c r="C6" s="43" t="inlineStr">
         <is>
-          <t>Corporate Office</t>
+          <t>Training Room</t>
         </is>
       </c>
       <c r="D6" s="34" t="n"/>
@@ -1727,11 +1727,7 @@
           <t>Corporate Office</t>
         </is>
       </c>
-      <c r="D36" s="74" t="inlineStr">
-        <is>
-          <t>✅</t>
-        </is>
-      </c>
+      <c r="D36" s="74" t="inlineStr"/>
       <c r="E36" s="8" t="inlineStr">
         <is>
           <t>Adityo Asmoro</t>
@@ -1809,7 +1805,11 @@
           <t>Training Room</t>
         </is>
       </c>
-      <c r="D38" s="74" t="inlineStr"/>
+      <c r="D38" s="74" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
       <c r="E38" s="8" t="inlineStr">
         <is>
           <t>Adityo Asmoro</t>

</xml_diff>